<commit_message>
Updated Summarized Age Graph
</commit_message>
<xml_diff>
--- a/Style_Guide.xlsx
+++ b/Style_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcclary\Documents\GitHub\Demographics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA59016D-0DD8-4797-A0B7-7AEDA1CC965D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA0EDD3-86C9-4087-B527-47804F2E7104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15720" xr2:uid="{74F6E861-9D85-4765-BF52-3E40BB1F16F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74F6E861-9D85-4765-BF52-3E40BB1F16F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,7 +639,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Median Income Graphs and Race
</commit_message>
<xml_diff>
--- a/Style_Guide.xlsx
+++ b/Style_Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcclary\Documents\GitHub\Demographics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA0EDD3-86C9-4087-B527-47804F2E7104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D5EB9C-B136-49BA-A6DD-312FF41C5F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74F6E861-9D85-4765-BF52-3E40BB1F16F7}"/>
   </bookViews>
@@ -204,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +274,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF4E3629"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7A4F06"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3E450A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8F893B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,11 +308,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -308,6 +325,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,6 +336,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF8F893B"/>
+      <color rgb="FF3E450A"/>
+      <color rgb="FF7A4F06"/>
       <color rgb="FF4E3629"/>
       <color rgb="FF0072CE"/>
       <color rgb="FF789D4A"/>
@@ -323,9 +346,6 @@
       <color rgb="FF80638F"/>
       <color rgb="FFD48500"/>
       <color rgb="FFB3AB4A"/>
-      <color rgb="FF9C301A"/>
-      <color rgb="FF00407A"/>
-      <color rgb="FF4D590D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -639,7 +659,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +693,7 @@
       <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="14" t="s">
         <v>37</v>
       </c>
       <c r="K2" s="1"/>
@@ -682,14 +702,14 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K3" s="1"/>
@@ -698,7 +718,7 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -708,14 +728,14 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="4"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -724,13 +744,13 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -745,8 +765,8 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -760,8 +780,8 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -775,8 +795,8 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -790,7 +810,7 @@
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
@@ -805,8 +825,8 @@
       <c r="A11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="12"/>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -815,12 +835,13 @@
       <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
Updated figures for census presentation
</commit_message>
<xml_diff>
--- a/Style_Guide.xlsx
+++ b/Style_Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amcclary\Documents\GitHub\Demographics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA3F0EF-A639-4AEC-9E7C-F6B4E13A9DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37713B69-698B-491A-B9D9-7213C8F9FA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{74F6E861-9D85-4765-BF52-3E40BB1F16F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74F6E861-9D85-4765-BF52-3E40BB1F16F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -659,7 +659,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>